<commit_message>
add slug and make view dynamic
</commit_message>
<xml_diff>
--- a/public/assets/frontend/example/types.xlsx
+++ b/public/assets/frontend/example/types.xlsx
@@ -20,18 +20,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t xml:space="preserve">name</t>
   </si>
   <si>
-    <t xml:space="preserve">one</t>
+    <t xml:space="preserve">slug</t>
   </si>
   <si>
-    <t xml:space="preserve">two</t>
+    <t xml:space="preserve">Camera</t>
   </si>
   <si>
-    <t xml:space="preserve">three</t>
+    <t xml:space="preserve">camera</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Recorder</t>
+  </si>
+  <si>
+    <t xml:space="preserve">recorder</t>
   </si>
 </sst>
 </file>
@@ -133,10 +139,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -145,21 +151,28 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" s="0" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>2</v>
+        <v>4</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
-        <v>3</v>
-      </c>
+      <c r="A4" s="1"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>